<commit_message>
add excel keyword auto reply
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minihorse/Desktop/webhook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63ACF559-8F32-B649-9D60-697C5FE3C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C55151-01FB-8E4B-8AEE-8D42C75BFE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="24820" windowHeight="14360" xr2:uid="{1082BAF5-4381-6B44-B304-BDC963BD07A8}"/>
+    <workbookView xWindow="3500" yWindow="1520" windowWidth="24820" windowHeight="14360" xr2:uid="{1082BAF5-4381-6B44-B304-BDC963BD07A8}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,43 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>哈囉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>您好～請問需要什麼協助？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>價格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>價格請參考賣貨便或蝦皮連結</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出貨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最晚明天出貨喔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>keyword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -392,12 +429,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90209C0-DD46-C444-978C-A45AA56AD415}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>